<commit_message>
updated all GSC export files
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>2025-11-06</t>
+  </si>
+  <si>
+    <t>2025-11-07</t>
   </si>
   <si>
     <t>Issue</t>
@@ -177,7 +180,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -544,6 +547,17 @@
       </c>
       <c r="C33" t="n" s="0">
         <v>95.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>87.0</v>
       </c>
     </row>
   </sheetData>
@@ -561,13 +575,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -585,13 +599,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GSC export files
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>2025-11-07</t>
+  </si>
+  <si>
+    <t>2025-11-08</t>
+  </si>
+  <si>
+    <t>2025-11-09</t>
   </si>
   <si>
     <t>Issue</t>
@@ -180,7 +186,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -558,6 +564,28 @@
       </c>
       <c r="C34" t="n" s="0">
         <v>87.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>76.0</v>
       </c>
     </row>
   </sheetData>
@@ -575,13 +603,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -599,13 +627,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GSC export data
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>2025-11-12</t>
+  </si>
+  <si>
+    <t>2025-11-13</t>
+  </si>
+  <si>
+    <t>2025-11-14</t>
   </si>
   <si>
     <t>Issue</t>
@@ -195,7 +201,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -628,6 +634,28 @@
       </c>
       <c r="C39" t="n" s="0">
         <v>43.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="B40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C41" t="n" s="0">
+        <v>38.0</v>
       </c>
     </row>
   </sheetData>
@@ -645,13 +673,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -669,13 +697,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated GSC data files for main domain
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>2025-11-15</t>
+  </si>
+  <si>
+    <t>2025-11-16</t>
   </si>
   <si>
     <t>Issue</t>
@@ -204,7 +207,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -670,6 +673,17 @@
       </c>
       <c r="C42" t="n" s="0">
         <v>35.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="B43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C43" t="n" s="0">
+        <v>31.0</v>
       </c>
     </row>
   </sheetData>
@@ -687,13 +701,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -711,13 +725,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated main GSC export data
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Date</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>2025-11-16</t>
+  </si>
+  <si>
+    <t>2025-11-17</t>
   </si>
   <si>
     <t>Issue</t>
@@ -207,7 +210,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -684,6 +687,17 @@
       </c>
       <c r="C43" t="n" s="0">
         <v>31.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C44" t="n" s="0">
+        <v>29.0</v>
       </c>
     </row>
   </sheetData>
@@ -701,13 +715,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -725,13 +739,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated main GSC export files
</commit_message>
<xml_diff>
--- a/gsc-export/Breadcrumbs.xlsx
+++ b/gsc-export/Breadcrumbs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
   <si>
     <t>Date</t>
   </si>
@@ -176,6 +176,21 @@
   </si>
   <si>
     <t>2025-11-25</t>
+  </si>
+  <si>
+    <t>2025-11-26</t>
+  </si>
+  <si>
+    <t>2025-11-27</t>
+  </si>
+  <si>
+    <t>2025-11-28</t>
+  </si>
+  <si>
+    <t>2025-11-29</t>
+  </si>
+  <si>
+    <t>2025-11-30</t>
   </si>
   <si>
     <t>Issue</t>
@@ -234,7 +249,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" rightToLeft="false"/>
   </sheetViews>
@@ -809,6 +824,61 @@
         <v>0.0</v>
       </c>
       <c r="C52" t="n" s="0">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="B53" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C53" t="n" s="0">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B54" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C54" t="n" s="0">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="B55" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C55" t="n" s="0">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B56" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C56" t="n" s="0">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="B57" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="C57" t="n" s="0">
         <v>27.0</v>
       </c>
     </row>
@@ -827,13 +897,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -851,13 +921,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>56</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>